<commit_message>
end of day check in
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template - Botanical Family test.xlsx
+++ b/data/Crop Rotation Sample Template - Botanical Family test.xlsx
@@ -776,7 +776,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D5" sqref="D5:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,7 +852,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -866,7 +866,7 @@
         <v>25</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -880,7 +880,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -894,7 +894,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -908,7 +908,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -922,7 +922,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -936,7 +936,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -954,7 +954,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X24" sqref="X24:X37"/>
+      <selection pane="bottomRight" activeCell="X47" sqref="X47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2181,7 +2181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -2230,10 +2230,10 @@
         <v>120</v>
       </c>
       <c r="X24" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
@@ -2282,10 +2282,10 @@
         <v>120</v>
       </c>
       <c r="X25" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
@@ -2334,10 +2334,10 @@
         <v>130</v>
       </c>
       <c r="X26" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>60</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>130</v>
       </c>
       <c r="X27" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
@@ -2919,7 +2919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>72</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>120</v>
       </c>
       <c r="X44" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
clean up of delta rotation variable generation
</commit_message>
<xml_diff>
--- a/data/Crop Rotation Sample Template - Botanical Family test.xlsx
+++ b/data/Crop Rotation Sample Template - Botanical Family test.xlsx
@@ -862,7 +862,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,7 +966,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,7 +980,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -994,7 +994,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1008,7 +1008,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1022,7 +1022,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1040,7 +1040,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="I41" sqref="I41:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3706,7 +3706,7 @@
   <mergeCells count="1">
     <mergeCell ref="K1:V1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:X10 A18:X51 A13:W13 A17:W17">
+  <conditionalFormatting sqref="A3:X10 A13:W13 A17:W17 A18:X51">
     <cfRule type="expression" dxfId="8" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>